<commit_message>
Changes to Login testcase
</commit_message>
<xml_diff>
--- a/Functional_Testing/TestDatas/LoginData.xlsx
+++ b/Functional_Testing/TestDatas/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\Desktop\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -127,12 +127,16 @@
   </si>
   <si>
     <t>$%@ga.com</t>
+  </si>
+  <si>
+    <t>Invalid parameters provided. Please provide valid parameters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,10 +573,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="87.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="64.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="64.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,7 +716,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -726,7 +730,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,7 +744,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,7 +800,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register and Contact Us code update
</commit_message>
<xml_diff>
--- a/Functional_Testing/TestDatas/LoginData.xlsx
+++ b/Functional_Testing/TestDatas/LoginData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="36">
   <si>
     <t>Email</t>
   </si>
@@ -130,6 +130,11 @@
   </si>
   <si>
     <t>Invalid parameters provided. Please provide valid parameters.</t>
+  </si>
+  <si>
+    <t>Profiles based on Bengaluru
+See all profiles from
+Bengaluru</t>
   </si>
 </sst>
 </file>
@@ -604,7 +609,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>